<commit_message>
update user & admin
</commit_message>
<xml_diff>
--- a/public/file/default_template.xlsx
+++ b/public/file/default_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sekolah\public\file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7AD32FC-92F3-4594-B164-9F16388EB342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A01FDA-8755-4C51-A2A3-BBE25A5865E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6525" yWindow="3090" windowWidth="20550" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="3420" windowWidth="20550" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="20">
   <si>
     <t>id</t>
   </si>
@@ -440,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="D11" sqref="D11:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,21 +537,282 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="1"/>
-      <c r="L3" s="2"/>
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>12345</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="1"/>
-      <c r="L4" s="2"/>
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>12345</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>12345</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>12345</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>12345</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>12345</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>12345</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" xr:uid="{71AB8E1B-8261-4DF5-A01E-F1A9A6D16680}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{77489C43-BC92-4D3E-B561-33AD4D3C185E}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{D4239798-A406-4DD3-BFE3-AA107AEC4413}"/>
+    <hyperlink ref="J5" r:id="rId4" xr:uid="{D52AF6DA-0FB5-4B04-8A53-5B935DC5C931}"/>
+    <hyperlink ref="J6" r:id="rId5" xr:uid="{8149CE5D-BE6D-4523-90F3-11D7B0AECFD4}"/>
+    <hyperlink ref="J7" r:id="rId6" xr:uid="{157A3F2B-A68A-4A8C-BC31-D260AC11BC95}"/>
+    <hyperlink ref="J9" r:id="rId7" xr:uid="{2CFB3CA7-734B-45F0-A576-5C0BCBB12FB4}"/>
+    <hyperlink ref="J8" r:id="rId8" xr:uid="{A40A867E-A433-42C3-BFB8-2864C159B08E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>